<commit_message>
first upload, union data, scraper
</commit_message>
<xml_diff>
--- a/union_data.xlsx
+++ b/union_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexBusch\Documents\GitHub\industrial_action\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B61C27D-1025-4A32-A847-8DBF752D68D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD7BE9E-44DB-4C88-A9C5-9B91E485D7F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10500" xr2:uid="{55DB6E5A-4C35-45C3-9C4F-265E93AFAEF7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="317">
   <si>
     <t>U-Union</t>
   </si>
@@ -57,12 +57,6 @@
     <t>https://netkey40.igmetall.de/homepages/aachen/</t>
   </si>
   <si>
-    <t>https://www.aalen.igm.de/</t>
-  </si>
-  <si>
-    <t>https://www.albstadt.igm.de/</t>
-  </si>
-  <si>
     <t>Alfeld-Hameln-Hildesheim</t>
   </si>
   <si>
@@ -78,18 +72,12 @@
     <t>url3</t>
   </si>
   <si>
-    <t>https://allgaeu.igmetall.de/</t>
-  </si>
-  <si>
     <t>Allgaeu</t>
   </si>
   <si>
     <t>url4</t>
   </si>
   <si>
-    <t>https://amberg.igmetall.de/</t>
-  </si>
-  <si>
     <t>Amberg</t>
   </si>
   <si>
@@ -108,9 +96,6 @@
     <t>url1</t>
   </si>
   <si>
-    <t>https://aschaffenburg.igmetall.de/</t>
-  </si>
-  <si>
     <t>Aschaffenburg</t>
   </si>
   <si>
@@ -126,9 +111,6 @@
     <t>Bad-Kreuznach</t>
   </si>
   <si>
-    <t>https://bamberg.igmetall.de/</t>
-  </si>
-  <si>
     <t>Bamberg</t>
   </si>
   <si>
@@ -171,15 +153,9 @@
     <t>Braunschweig</t>
   </si>
   <si>
-    <t>https://bremen.igmetall.de/</t>
-  </si>
-  <si>
     <t>Bremen</t>
   </si>
   <si>
-    <t>https://www.bruchsal.igm.de/</t>
-  </si>
-  <si>
     <t>Bruchsal</t>
   </si>
   <si>
@@ -246,36 +222,21 @@
     <t>Erfurt</t>
   </si>
   <si>
-    <t>https://erlangen.igmetall.de/</t>
-  </si>
-  <si>
     <t>Erlangen</t>
   </si>
   <si>
-    <t>https://www.esslingen.igm.de/</t>
-  </si>
-  <si>
     <t>Esslingen</t>
   </si>
   <si>
-    <t>https://flensburg.igmetall.de/</t>
-  </si>
-  <si>
     <t>Frankfurt</t>
   </si>
   <si>
     <t>Flensburg</t>
   </si>
   <si>
-    <t>https://www.freiburg.igm.de/</t>
-  </si>
-  <si>
     <t>Freiburg</t>
   </si>
   <si>
-    <t>https://www.freudenstadt.igm.de/</t>
-  </si>
-  <si>
     <t>Freudenstadt</t>
   </si>
   <si>
@@ -285,9 +246,6 @@
     <t>Friedrichshafen-Oberschwaben</t>
   </si>
   <si>
-    <t>https://www.gaggenau.igm.de/</t>
-  </si>
-  <si>
     <t>Gaggenau</t>
   </si>
   <si>
@@ -300,9 +258,6 @@
     <t>Jena-Saalfeld-Gera</t>
   </si>
   <si>
-    <t>https://www.goeppingen-geislingen.igm.de/</t>
-  </si>
-  <si>
     <t>Goeppingen-Geislingen</t>
   </si>
   <si>
@@ -363,21 +318,12 @@
     <t>url13</t>
   </si>
   <si>
-    <t>https://www.heidelberg.igm.de/</t>
-  </si>
-  <si>
     <t>Heidelberg</t>
   </si>
   <si>
-    <t>https://www.heidenheim.igm.de/</t>
-  </si>
-  <si>
     <t>Heidenheim</t>
   </si>
   <si>
-    <t>https://www.neckarsulm.igm.de/</t>
-  </si>
-  <si>
     <t>Heilbronn-Neckarsulm</t>
   </si>
   <si>
@@ -417,15 +363,9 @@
     <t>Kaiserslautern</t>
   </si>
   <si>
-    <t>https://www.karlsruhe.igm.de/</t>
-  </si>
-  <si>
     <t>Karlsruhe</t>
   </si>
   <si>
-    <t>https://kiel-neumuenster.igmetall.de/</t>
-  </si>
-  <si>
     <t>Kiel-Neumuenster</t>
   </si>
   <si>
@@ -474,15 +414,9 @@
     <t>url14</t>
   </si>
   <si>
-    <t>https://www.loerrach.igm.de/</t>
-  </si>
-  <si>
     <t>Loerrach</t>
   </si>
   <si>
-    <t>https://luebeck-wismar.igmetall.de/</t>
-  </si>
-  <si>
     <t>Luebeck-Wismar</t>
   </si>
   <si>
@@ -513,9 +447,6 @@
     <t>Mainz-Wiesbaden</t>
   </si>
   <si>
-    <t>https://www.mannheim.igm.de/</t>
-  </si>
-  <si>
     <t>Mannheim</t>
   </si>
   <si>
@@ -549,15 +480,9 @@
     <t>Muelheim-Essen-Oberhausen</t>
   </si>
   <si>
-    <t>https://www.offenburg.igm.de/</t>
-  </si>
-  <si>
     <t>Offenburg</t>
   </si>
   <si>
-    <t>https://oldenburg-wilhelmshaven.igmetall.de/</t>
-  </si>
-  <si>
     <t>Oldenburg-Wilhelmshaven</t>
   </si>
   <si>
@@ -594,9 +519,6 @@
     <t>Offenbach</t>
   </si>
   <si>
-    <t>https://olpe.igmetall.de/</t>
-  </si>
-  <si>
     <t>Olpe</t>
   </si>
   <si>
@@ -621,9 +543,6 @@
     <t>Ostbrandenburg</t>
   </si>
   <si>
-    <t>https://ostoberfranken.igmetall.de/</t>
-  </si>
-  <si>
     <t>Oberfranken</t>
   </si>
   <si>
@@ -654,9 +573,6 @@
     <t>url23</t>
   </si>
   <si>
-    <t>https://regensburg.igmetall.de/</t>
-  </si>
-  <si>
     <t>Regensburg</t>
   </si>
   <si>
@@ -675,15 +591,9 @@
     <t>url24</t>
   </si>
   <si>
-    <t>https://rendsburg.igmetall.de/</t>
-  </si>
-  <si>
     <t>Rendsburg</t>
   </si>
   <si>
-    <t>https://www.reutlingen.igm.de/</t>
-  </si>
-  <si>
     <t>Reutlingen-Tuebingen</t>
   </si>
   <si>
@@ -705,9 +615,6 @@
     <t>Rosenheim</t>
   </si>
   <si>
-    <t>https://rostock-schwerin.igmetall.de/</t>
-  </si>
-  <si>
     <t>Rostock-Schwerin</t>
   </si>
   <si>
@@ -741,21 +648,12 @@
     <t>Schwabach</t>
   </si>
   <si>
-    <t>https://www.schwaebisch-gmuend.igm.de/</t>
-  </si>
-  <si>
     <t>Schwaebisch-Gmuend</t>
   </si>
   <si>
-    <t>https://www.schwaebisch-hall.igm.de/</t>
-  </si>
-  <si>
     <t>Schaebisch-Hall</t>
   </si>
   <si>
-    <t>https://schweinfurt.igmetall.de/</t>
-  </si>
-  <si>
     <t>Schweinfurt</t>
   </si>
   <si>
@@ -765,9 +663,6 @@
     <t>Siegen</t>
   </si>
   <si>
-    <t>https://www.singen.igm.de/</t>
-  </si>
-  <si>
     <t>Singen</t>
   </si>
   <si>
@@ -777,9 +672,6 @@
     <t>Stralsund-Neubrandenburg</t>
   </si>
   <si>
-    <t>https://www.stuttgart.igm.de/</t>
-  </si>
-  <si>
     <t>Stuttgart</t>
   </si>
   <si>
@@ -795,18 +687,12 @@
     <t>Suehl-Sonneberg</t>
   </si>
   <si>
-    <t>https://www.tauberbischofsheim.igm.de/</t>
-  </si>
-  <si>
     <t>Tauberbischofsheim</t>
   </si>
   <si>
     <t>Trier</t>
   </si>
   <si>
-    <t>https://www.ulm.igm.de/</t>
-  </si>
-  <si>
     <t>Ulm</t>
   </si>
   <si>
@@ -816,9 +702,6 @@
     <t>Unna</t>
   </si>
   <si>
-    <t>https://unterelbe.igmetall.de/</t>
-  </si>
-  <si>
     <t>Unterelbe</t>
   </si>
   <si>
@@ -831,18 +714,12 @@
     <t>url26</t>
   </si>
   <si>
-    <t>https://www.villingen-schwenningen.igm.de/</t>
-  </si>
-  <si>
     <t>Villingen-Schwenningen</t>
   </si>
   <si>
     <t>Voelklingen</t>
   </si>
   <si>
-    <t>https://weilheim.igmetall.de/</t>
-  </si>
-  <si>
     <t>Weilheim</t>
   </si>
   <si>
@@ -852,15 +729,9 @@
     <t>Weser-Elbe</t>
   </si>
   <si>
-    <t>https://wesermarsch.igmetall.de/</t>
-  </si>
-  <si>
     <t>Wesermarsch</t>
   </si>
   <si>
-    <t>https://westmittelfranken.igmetall.de/</t>
-  </si>
-  <si>
     <t>Westmittelfranken</t>
   </si>
   <si>
@@ -964,6 +835,147 @@
   </si>
   <si>
     <t>https://www.igmetall-voelklingen.de/news/meldungsarchiv/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no news? </t>
+  </si>
+  <si>
+    <t>https://aschaffenburg.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://amberg.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://allgaeu.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://www.aalen.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.albstadt.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.bruchsal.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.esslingen.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.freiburg.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.freudenstadt.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.gaggenau.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.villingen-schwenningen.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.ulm.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.tauberbischofsheim.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.stuttgart.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.singen.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.schwaebisch-hall.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.schwaebisch-gmuend.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.reutlingen.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.offenburg.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.mannheim.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.loerrach.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.karlsruhe.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.neckarsulm.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.heidenheim.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.heidelberg.igm.de/news/</t>
+  </si>
+  <si>
+    <t>https://www.goeppingen-geislingen.igm.de/news/</t>
+  </si>
+  <si>
+    <t>urlby1</t>
+  </si>
+  <si>
+    <t>urlby2</t>
+  </si>
+  <si>
+    <t>https://flensburg.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://kiel-neumuenster.igmetall.de/aktuelle-meldungen</t>
+  </si>
+  <si>
+    <t>https://luebeck-wismar.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://oldenburg-wilhelmshaven.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://olpe.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://ostoberfranken.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://regensburg.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://rendsburg.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://rostock-schwerin.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://erlangen.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://bremen.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://bamberg.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://schweinfurt.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://unterelbe.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unsure whether same structure </t>
+  </si>
+  <si>
+    <t>https://weilheim.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://wesermarsch.igmetall.de/aktuell</t>
+  </si>
+  <si>
+    <t>https://westmittelfranken.igmetall.de/aktuell</t>
   </si>
 </sst>
 </file>
@@ -1329,13 +1341,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF38B2E-D1B8-4839-8784-A9099D704EE1}">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,7 +1364,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1369,7 +1381,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1380,13 +1392,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>274</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1396,14 +1408,14 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
+      <c r="C4" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1414,13 +1426,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1431,13 +1443,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>273</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1448,13 +1460,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>272</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1465,13 +1477,13 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1481,14 +1493,14 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
+      <c r="C9" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1499,13 +1511,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>298</v>
+      </c>
+      <c r="F10" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1516,13 +1531,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>286</v>
+        <v>243</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1533,13 +1548,13 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>310</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1550,13 +1565,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1567,13 +1582,13 @@
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>287</v>
+        <v>244</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1584,13 +1599,13 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1601,13 +1616,13 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1618,13 +1633,13 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1635,13 +1650,13 @@
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>288</v>
+        <v>245</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1651,14 +1666,14 @@
       <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
-        <v>48</v>
+      <c r="C19" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1668,14 +1683,14 @@
       <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
-        <v>50</v>
+      <c r="C20" s="1" t="s">
+        <v>276</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1686,13 +1701,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1703,13 +1718,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1720,13 +1735,13 @@
         <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1737,13 +1752,13 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1754,13 +1769,13 @@
         <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>289</v>
+        <v>246</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1771,13 +1786,13 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1788,13 +1803,13 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1805,13 +1820,13 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1822,13 +1837,13 @@
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>290</v>
+        <v>247</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1839,13 +1854,13 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1856,13 +1871,13 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,13 +1888,13 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>297</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1890,13 +1905,13 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1907,13 +1922,13 @@
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>291</v>
+        <v>248</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1924,13 +1939,13 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>308</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1940,14 +1955,14 @@
       <c r="B36" t="s">
         <v>3</v>
       </c>
-      <c r="C36" t="s">
-        <v>75</v>
+      <c r="C36" s="1" t="s">
+        <v>277</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1958,13 +1973,13 @@
         <v>3</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>77</v>
+        <v>299</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E37" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1975,13 +1990,13 @@
         <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1991,14 +2006,14 @@
       <c r="B39" t="s">
         <v>3</v>
       </c>
-      <c r="C39" t="s">
-        <v>80</v>
+      <c r="C39" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2008,14 +2023,14 @@
       <c r="B40" t="s">
         <v>3</v>
       </c>
-      <c r="C40" t="s">
-        <v>82</v>
+      <c r="C40" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2026,10 +2041,10 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2039,14 +2054,14 @@
       <c r="B42" t="s">
         <v>3</v>
       </c>
-      <c r="C42" t="s">
-        <v>86</v>
+      <c r="C42" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="D42" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2057,13 +2072,13 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E43" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2074,13 +2089,13 @@
         <v>3</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2090,14 +2105,14 @@
       <c r="B45" t="s">
         <v>3</v>
       </c>
-      <c r="C45" t="s">
-        <v>91</v>
+      <c r="C45" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="D45" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2108,16 +2123,16 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E46" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F46" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2128,13 +2143,13 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E47" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2145,13 +2160,13 @@
         <v>3</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E48" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2162,16 +2177,16 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D49" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E49" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="F49" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2182,13 +2197,13 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="D50" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E50" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2199,13 +2214,13 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D51" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E51" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2216,13 +2231,13 @@
         <v>3</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="D52" t="s">
         <v>4</v>
       </c>
       <c r="E52" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2233,13 +2248,13 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D53" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="E53" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2249,14 +2264,14 @@
       <c r="B54" t="s">
         <v>3</v>
       </c>
-      <c r="C54" t="s">
-        <v>112</v>
+      <c r="C54" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="D54" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E54" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2266,14 +2281,14 @@
       <c r="B55" t="s">
         <v>3</v>
       </c>
-      <c r="C55" t="s">
-        <v>114</v>
+      <c r="C55" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="D55" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2283,14 +2298,14 @@
       <c r="B56" t="s">
         <v>3</v>
       </c>
-      <c r="C56" t="s">
-        <v>116</v>
+      <c r="C56" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="D56" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="E56" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2301,13 +2316,13 @@
         <v>3</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>296</v>
+        <v>253</v>
       </c>
       <c r="D57" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="E57" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2318,13 +2333,13 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="D58" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="E58" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2335,13 +2350,13 @@
         <v>3</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="D59" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="E59" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2352,13 +2367,13 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="D60" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="E60" t="s">
-        <v>35</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2369,13 +2384,13 @@
         <v>3</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="D61" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="E61" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2385,14 +2400,14 @@
       <c r="B62" t="s">
         <v>3</v>
       </c>
-      <c r="C62" t="s">
-        <v>130</v>
+      <c r="C62" s="1" t="s">
+        <v>292</v>
       </c>
       <c r="D62" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2403,13 +2418,13 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>132</v>
+        <v>300</v>
       </c>
       <c r="D63" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="E63" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2420,13 +2435,13 @@
         <v>3</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>299</v>
+        <v>256</v>
       </c>
       <c r="D64" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="E64" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2437,13 +2452,13 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="D65" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="E65" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2454,13 +2469,13 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="D66" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="E66" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -2471,13 +2486,13 @@
         <v>3</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="E67" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2488,13 +2503,13 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="D68" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="E68" t="s">
-        <v>35</v>
+        <v>297</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2505,13 +2520,13 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="D69" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="E69" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2522,13 +2537,13 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="D70" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="E70" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2538,14 +2553,14 @@
       <c r="B71" t="s">
         <v>3</v>
       </c>
-      <c r="C71" t="s">
-        <v>149</v>
+      <c r="C71" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="D71" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="E71" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -2556,13 +2571,13 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>301</v>
       </c>
       <c r="D72" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="E72" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2573,13 +2588,13 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="D73" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="E73" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -2590,13 +2605,13 @@
         <v>3</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="D74" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="E74" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2607,13 +2622,13 @@
         <v>3</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>301</v>
+        <v>258</v>
       </c>
       <c r="D75" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="E75" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -2624,13 +2639,13 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="D76" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="E76" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2641,13 +2656,13 @@
         <v>3</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>302</v>
+        <v>259</v>
       </c>
       <c r="D77" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="E77" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2657,14 +2672,14 @@
       <c r="B78" t="s">
         <v>3</v>
       </c>
-      <c r="C78" t="s">
-        <v>162</v>
+      <c r="C78" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="D78" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="E78" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2675,13 +2690,13 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="D79" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="E79" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2692,13 +2707,13 @@
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="D80" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="E80" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2709,13 +2724,13 @@
         <v>3</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="D81" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E81" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2726,13 +2741,13 @@
         <v>3</v>
       </c>
       <c r="C82" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="D82" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="E82" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2743,13 +2758,13 @@
         <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="D83" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="E83" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2759,14 +2774,14 @@
       <c r="B84" t="s">
         <v>3</v>
       </c>
-      <c r="C84" t="s">
-        <v>174</v>
+      <c r="C84" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="D84" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="E84" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2777,13 +2792,13 @@
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>176</v>
+        <v>302</v>
       </c>
       <c r="D85" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="E85" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2794,13 +2809,13 @@
         <v>3</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>304</v>
+        <v>261</v>
       </c>
       <c r="D86" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="E86" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2811,13 +2826,13 @@
         <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="D87" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="E87" t="s">
-        <v>35</v>
+        <v>297</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2828,13 +2843,13 @@
         <v>3</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>305</v>
+        <v>262</v>
       </c>
       <c r="D88" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="E88" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2845,13 +2860,13 @@
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="D89" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="E89" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -2862,13 +2877,13 @@
         <v>3</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="D90" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="E90" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -2879,13 +2894,13 @@
         <v>3</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
       <c r="D91" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="E91" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2896,13 +2911,13 @@
         <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="D92" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="E92" t="s">
-        <v>35</v>
+        <v>297</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -2913,13 +2928,13 @@
         <v>3</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>308</v>
+        <v>265</v>
       </c>
       <c r="D93" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="E93" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -2930,13 +2945,13 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>189</v>
+        <v>303</v>
       </c>
       <c r="D94" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="E94" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -2947,13 +2962,13 @@
         <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="D95" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="E95" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -2964,16 +2979,16 @@
         <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="D96" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="E96" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2981,16 +2996,16 @@
         <v>3</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>309</v>
+        <v>266</v>
       </c>
       <c r="D97" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="E97" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2998,16 +3013,16 @@
         <v>3</v>
       </c>
       <c r="C98" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="D98" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="E98" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3015,16 +3030,16 @@
         <v>3</v>
       </c>
       <c r="C99" t="s">
-        <v>198</v>
+        <v>304</v>
       </c>
       <c r="D99" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="E99" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3032,16 +3047,16 @@
         <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="D100" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="E100" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3049,16 +3064,16 @@
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="D101" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="E101" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3066,16 +3081,19 @@
         <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="D102" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="E102" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="F102" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3083,16 +3101,16 @@
         <v>3</v>
       </c>
       <c r="C103" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="D103" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="E103" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3100,16 +3118,16 @@
         <v>3</v>
       </c>
       <c r="C104" t="s">
-        <v>209</v>
+        <v>305</v>
       </c>
       <c r="D104" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="E104" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3117,16 +3135,16 @@
         <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="D105" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="E105" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3134,16 +3152,16 @@
         <v>3</v>
       </c>
       <c r="C106" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="D106" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="E106" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3151,33 +3169,33 @@
         <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>216</v>
+        <v>306</v>
       </c>
       <c r="D107" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="E107" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>3</v>
       </c>
-      <c r="C108" t="s">
-        <v>218</v>
+      <c r="C108" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="D108" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="E108" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3185,16 +3203,16 @@
         <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="D109" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="E109" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3202,16 +3220,16 @@
         <v>3</v>
       </c>
       <c r="C110" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="D110" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="E110" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3219,16 +3237,16 @@
         <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="D111" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="E111" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3236,13 +3254,13 @@
         <v>3</v>
       </c>
       <c r="C112" t="s">
-        <v>226</v>
+        <v>307</v>
       </c>
       <c r="D112" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="E112" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3253,16 +3271,16 @@
         <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="D113" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="E113" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="F113" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3273,13 +3291,13 @@
         <v>3</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="D114" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="E114" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3290,13 +3308,13 @@
         <v>3</v>
       </c>
       <c r="C115" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="D115" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="E115" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3307,13 +3325,16 @@
         <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="D116" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="E116" t="s">
-        <v>35</v>
+        <v>298</v>
+      </c>
+      <c r="F116" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3323,14 +3344,14 @@
       <c r="B117" t="s">
         <v>3</v>
       </c>
-      <c r="C117" t="s">
-        <v>238</v>
+      <c r="C117" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="D117" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="E117" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3340,14 +3361,14 @@
       <c r="B118" t="s">
         <v>3</v>
       </c>
-      <c r="C118" t="s">
-        <v>240</v>
+      <c r="C118" s="1" t="s">
+        <v>286</v>
       </c>
       <c r="D118" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="E118" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3358,13 +3379,13 @@
         <v>3</v>
       </c>
       <c r="C119" t="s">
-        <v>242</v>
+        <v>311</v>
       </c>
       <c r="D119" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
       <c r="E119" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3375,13 +3396,13 @@
         <v>3</v>
       </c>
       <c r="C120" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="D120" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="E120" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3391,14 +3412,14 @@
       <c r="B121" t="s">
         <v>3</v>
       </c>
-      <c r="C121" t="s">
-        <v>246</v>
+      <c r="C121" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="D121" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="E121" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3409,13 +3430,13 @@
         <v>3</v>
       </c>
       <c r="C122" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="D122" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="E122" t="s">
-        <v>35</v>
+        <v>297</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3425,14 +3446,14 @@
       <c r="B123" t="s">
         <v>3</v>
       </c>
-      <c r="C123" t="s">
-        <v>250</v>
+      <c r="C123" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="D123" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="E123" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3443,13 +3464,13 @@
         <v>3</v>
       </c>
       <c r="C124" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="D124" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="E124" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3460,13 +3481,13 @@
         <v>3</v>
       </c>
       <c r="C125" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="D125" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="E125" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3476,14 +3497,14 @@
       <c r="B126" t="s">
         <v>3</v>
       </c>
-      <c r="C126" t="s">
-        <v>256</v>
+      <c r="C126" s="1" t="s">
+        <v>283</v>
       </c>
       <c r="D126" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
       <c r="E126" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3494,13 +3515,13 @@
         <v>3</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>311</v>
+        <v>268</v>
       </c>
       <c r="D127" t="s">
-        <v>258</v>
+        <v>221</v>
       </c>
       <c r="E127" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3510,17 +3531,17 @@
       <c r="B128" t="s">
         <v>3</v>
       </c>
-      <c r="C128" t="s">
-        <v>259</v>
+      <c r="C128" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="D128" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="E128" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3528,16 +3549,16 @@
         <v>3</v>
       </c>
       <c r="C129" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="D129" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="E129" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3545,16 +3566,19 @@
         <v>3</v>
       </c>
       <c r="C130" t="s">
-        <v>263</v>
+        <v>312</v>
       </c>
       <c r="D130" t="s">
-        <v>264</v>
+        <v>225</v>
       </c>
       <c r="E130" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F130" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3562,33 +3586,33 @@
         <v>3</v>
       </c>
       <c r="C131" t="s">
-        <v>265</v>
+        <v>226</v>
       </c>
       <c r="D131" t="s">
-        <v>266</v>
+        <v>227</v>
       </c>
       <c r="E131" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
       <c r="B132" t="s">
         <v>3</v>
       </c>
-      <c r="C132" t="s">
-        <v>268</v>
+      <c r="C132" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="D132" t="s">
-        <v>269</v>
+        <v>229</v>
       </c>
       <c r="E132" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3596,16 +3620,16 @@
         <v>3</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="D133" t="s">
-        <v>270</v>
+        <v>230</v>
       </c>
       <c r="E133" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3613,16 +3637,16 @@
         <v>3</v>
       </c>
       <c r="C134" t="s">
-        <v>271</v>
+        <v>314</v>
       </c>
       <c r="D134" t="s">
-        <v>272</v>
+        <v>231</v>
       </c>
       <c r="E134" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3630,16 +3654,16 @@
         <v>3</v>
       </c>
       <c r="C135" t="s">
-        <v>273</v>
+        <v>232</v>
       </c>
       <c r="D135" t="s">
-        <v>274</v>
+        <v>233</v>
       </c>
       <c r="E135" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3647,16 +3671,16 @@
         <v>3</v>
       </c>
       <c r="C136" t="s">
-        <v>275</v>
+        <v>315</v>
       </c>
       <c r="D136" t="s">
-        <v>276</v>
+        <v>234</v>
       </c>
       <c r="E136" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3664,16 +3688,16 @@
         <v>3</v>
       </c>
       <c r="C137" t="s">
-        <v>277</v>
+        <v>316</v>
       </c>
       <c r="D137" t="s">
-        <v>278</v>
+        <v>235</v>
       </c>
       <c r="E137" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3681,16 +3705,16 @@
         <v>3</v>
       </c>
       <c r="C138" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
       <c r="D138" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="E138" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3698,16 +3722,16 @@
         <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="D139" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="E139" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3715,49 +3739,70 @@
         <v>3</v>
       </c>
       <c r="C140" t="s">
-        <v>284</v>
+        <v>241</v>
       </c>
       <c r="D140" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="E140" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C37" r:id="rId1" xr:uid="{9EF97FA3-9762-4CB9-89F8-09C280C254EB}"/>
-    <hyperlink ref="C23" r:id="rId2" xr:uid="{1D55898C-4F2D-4C0E-A008-438FFE5757C2}"/>
-    <hyperlink ref="C22" r:id="rId3" xr:uid="{7D0EDC23-B6B4-424D-BE3C-5504B6BEE94F}"/>
-    <hyperlink ref="C21" r:id="rId4" xr:uid="{084D4D62-3E32-4E56-A49E-D9FD2910E935}"/>
-    <hyperlink ref="C11" r:id="rId5" xr:uid="{71A6CA32-5BE0-499C-A09F-18CB0D14BDD1}"/>
-    <hyperlink ref="C14" r:id="rId6" xr:uid="{0DC27EAF-1FFB-4549-8CC3-23F0B16F100E}"/>
-    <hyperlink ref="C18" r:id="rId7" xr:uid="{E9458462-4BB7-45B6-BD01-03212CCA2011}"/>
-    <hyperlink ref="C25" r:id="rId8" xr:uid="{52FB9CCF-F3A3-4508-B265-B9A16B548A16}"/>
-    <hyperlink ref="C29" r:id="rId9" xr:uid="{FCE70F01-ACB6-417A-851B-875462CDCEC1}"/>
-    <hyperlink ref="C34" r:id="rId10" xr:uid="{631D216A-E606-41C0-A9DC-7CE4F4F2178F}"/>
-    <hyperlink ref="C38" r:id="rId11" xr:uid="{16008171-E71B-4195-AAED-EE5D63EC8FAD}"/>
-    <hyperlink ref="C44" r:id="rId12" xr:uid="{1F619A34-17D8-4242-8D8F-81DA12B368DA}"/>
-    <hyperlink ref="C48" r:id="rId13" xr:uid="{06424DEF-18C4-41DE-93B9-2934AC1DAD4A}"/>
-    <hyperlink ref="C52" r:id="rId14" xr:uid="{0F85CBB3-EAF2-439C-A897-6199EB9B0898}"/>
-    <hyperlink ref="C57" r:id="rId15" xr:uid="{10C6FB81-7248-4A40-B681-30A58147A34F}"/>
-    <hyperlink ref="C59" r:id="rId16" xr:uid="{06153331-EFAF-4AF9-BBD3-96E5CA4C7A60}"/>
-    <hyperlink ref="C61" r:id="rId17" xr:uid="{C6C2295E-BD9B-4346-9A9D-ED8D07A243EF}"/>
-    <hyperlink ref="C64" r:id="rId18" xr:uid="{64A7A1E6-52BC-4C21-BDD5-B9696D405E82}"/>
-    <hyperlink ref="C67" r:id="rId19" xr:uid="{76EEFD13-22CB-4139-8263-2F2986F90965}"/>
-    <hyperlink ref="C74" r:id="rId20" xr:uid="{251D81FE-761E-4AA5-945E-113B12680D81}"/>
-    <hyperlink ref="C75" r:id="rId21" xr:uid="{6AD2EA75-DF93-4A05-9D05-9A18F061A376}"/>
-    <hyperlink ref="C77" r:id="rId22" xr:uid="{885E4273-4836-4C52-8CF6-46996BC68CE8}"/>
-    <hyperlink ref="C81" r:id="rId23" xr:uid="{1920D51F-FB1A-46AD-AA2C-D33BF1709B91}"/>
-    <hyperlink ref="C86" r:id="rId24" xr:uid="{1854EF3F-6E69-4D17-B7EA-F60E5748DD02}"/>
-    <hyperlink ref="C88" r:id="rId25" xr:uid="{9F0F6481-ABE5-4F4A-894A-0F0F7A8A1BB1}"/>
-    <hyperlink ref="C90" r:id="rId26" xr:uid="{7EA9F407-5A92-445B-B0D4-99EF2E534E18}"/>
-    <hyperlink ref="C91" r:id="rId27" xr:uid="{84AE1136-F592-426F-933B-AFB37D5F27E2}"/>
-    <hyperlink ref="C93" r:id="rId28" xr:uid="{77D0C496-04B7-4A96-BD42-B0A5EBABB068}"/>
-    <hyperlink ref="C97" r:id="rId29" xr:uid="{536AAD99-A084-4A7F-9747-E843EB5F4D07}"/>
-    <hyperlink ref="C114" r:id="rId30" xr:uid="{AA9729B9-E53A-47AA-AEED-C0E4537E429B}"/>
-    <hyperlink ref="C127" r:id="rId31" xr:uid="{39218BE5-6D13-42B0-88EC-7FD8428E4F55}"/>
-    <hyperlink ref="C133" r:id="rId32" xr:uid="{63897912-784D-4376-A333-16118A2AB84A}"/>
+    <hyperlink ref="C23" r:id="rId1" xr:uid="{1D55898C-4F2D-4C0E-A008-438FFE5757C2}"/>
+    <hyperlink ref="C22" r:id="rId2" xr:uid="{7D0EDC23-B6B4-424D-BE3C-5504B6BEE94F}"/>
+    <hyperlink ref="C21" r:id="rId3" xr:uid="{084D4D62-3E32-4E56-A49E-D9FD2910E935}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{71A6CA32-5BE0-499C-A09F-18CB0D14BDD1}"/>
+    <hyperlink ref="C14" r:id="rId5" xr:uid="{0DC27EAF-1FFB-4549-8CC3-23F0B16F100E}"/>
+    <hyperlink ref="C18" r:id="rId6" xr:uid="{E9458462-4BB7-45B6-BD01-03212CCA2011}"/>
+    <hyperlink ref="C25" r:id="rId7" xr:uid="{52FB9CCF-F3A3-4508-B265-B9A16B548A16}"/>
+    <hyperlink ref="C29" r:id="rId8" xr:uid="{FCE70F01-ACB6-417A-851B-875462CDCEC1}"/>
+    <hyperlink ref="C34" r:id="rId9" xr:uid="{631D216A-E606-41C0-A9DC-7CE4F4F2178F}"/>
+    <hyperlink ref="C38" r:id="rId10" xr:uid="{16008171-E71B-4195-AAED-EE5D63EC8FAD}"/>
+    <hyperlink ref="C44" r:id="rId11" xr:uid="{1F619A34-17D8-4242-8D8F-81DA12B368DA}"/>
+    <hyperlink ref="C48" r:id="rId12" xr:uid="{06424DEF-18C4-41DE-93B9-2934AC1DAD4A}"/>
+    <hyperlink ref="C52" r:id="rId13" xr:uid="{0F85CBB3-EAF2-439C-A897-6199EB9B0898}"/>
+    <hyperlink ref="C57" r:id="rId14" xr:uid="{10C6FB81-7248-4A40-B681-30A58147A34F}"/>
+    <hyperlink ref="C59" r:id="rId15" xr:uid="{06153331-EFAF-4AF9-BBD3-96E5CA4C7A60}"/>
+    <hyperlink ref="C61" r:id="rId16" xr:uid="{C6C2295E-BD9B-4346-9A9D-ED8D07A243EF}"/>
+    <hyperlink ref="C64" r:id="rId17" xr:uid="{64A7A1E6-52BC-4C21-BDD5-B9696D405E82}"/>
+    <hyperlink ref="C67" r:id="rId18" xr:uid="{76EEFD13-22CB-4139-8263-2F2986F90965}"/>
+    <hyperlink ref="C74" r:id="rId19" xr:uid="{251D81FE-761E-4AA5-945E-113B12680D81}"/>
+    <hyperlink ref="C75" r:id="rId20" xr:uid="{6AD2EA75-DF93-4A05-9D05-9A18F061A376}"/>
+    <hyperlink ref="C77" r:id="rId21" xr:uid="{885E4273-4836-4C52-8CF6-46996BC68CE8}"/>
+    <hyperlink ref="C81" r:id="rId22" xr:uid="{1920D51F-FB1A-46AD-AA2C-D33BF1709B91}"/>
+    <hyperlink ref="C86" r:id="rId23" xr:uid="{1854EF3F-6E69-4D17-B7EA-F60E5748DD02}"/>
+    <hyperlink ref="C88" r:id="rId24" xr:uid="{9F0F6481-ABE5-4F4A-894A-0F0F7A8A1BB1}"/>
+    <hyperlink ref="C90" r:id="rId25" xr:uid="{7EA9F407-5A92-445B-B0D4-99EF2E534E18}"/>
+    <hyperlink ref="C91" r:id="rId26" xr:uid="{84AE1136-F592-426F-933B-AFB37D5F27E2}"/>
+    <hyperlink ref="C93" r:id="rId27" xr:uid="{77D0C496-04B7-4A96-BD42-B0A5EBABB068}"/>
+    <hyperlink ref="C97" r:id="rId28" xr:uid="{536AAD99-A084-4A7F-9747-E843EB5F4D07}"/>
+    <hyperlink ref="C114" r:id="rId29" xr:uid="{AA9729B9-E53A-47AA-AEED-C0E4537E429B}"/>
+    <hyperlink ref="C127" r:id="rId30" xr:uid="{39218BE5-6D13-42B0-88EC-7FD8428E4F55}"/>
+    <hyperlink ref="C133" r:id="rId31" xr:uid="{63897912-784D-4376-A333-16118A2AB84A}"/>
+    <hyperlink ref="C4" r:id="rId32" xr:uid="{08E7118B-941A-4EE5-81DA-9DFA11E06E99}"/>
+    <hyperlink ref="C20" r:id="rId33" xr:uid="{2E3C695B-8316-4C5A-8654-856A0971A4F1}"/>
+    <hyperlink ref="C36" r:id="rId34" xr:uid="{A699AD30-C7D2-4E20-B183-3E56852EAC56}"/>
+    <hyperlink ref="C39" r:id="rId35" xr:uid="{99601A63-A147-445F-B354-2ADB7A19285E}"/>
+    <hyperlink ref="C40" r:id="rId36" xr:uid="{42F2B40B-3896-4D86-8E1F-D1E66A687444}"/>
+    <hyperlink ref="C42" r:id="rId37" xr:uid="{2AF3065E-C515-43E8-9C34-394857DEDF99}"/>
+    <hyperlink ref="C132" r:id="rId38" xr:uid="{BCDEBE63-B57B-43A8-AF62-602F20CAFE86}"/>
+    <hyperlink ref="C128" r:id="rId39" xr:uid="{1E1B47C2-0536-488B-B3B3-FF62383B6F35}"/>
+    <hyperlink ref="C126" r:id="rId40" xr:uid="{ABE47253-802C-438C-8EBF-8B9A3C616B04}"/>
+    <hyperlink ref="C123" r:id="rId41" xr:uid="{783E043C-B8E7-4321-9DF8-F25369B4E2BE}"/>
+    <hyperlink ref="C121" r:id="rId42" xr:uid="{9DC00A52-D7A7-426E-9B24-F2D24D5CAAEA}"/>
+    <hyperlink ref="C118" r:id="rId43" xr:uid="{B85A2729-83A3-4620-9BBB-38B65B533BF3}"/>
+    <hyperlink ref="C117" r:id="rId44" xr:uid="{565BF175-4242-44DA-A997-E2A48218ECF0}"/>
+    <hyperlink ref="C108" r:id="rId45" xr:uid="{1AC2C38E-F15D-4D95-887A-284DF240403C}"/>
+    <hyperlink ref="C84" r:id="rId46" xr:uid="{9946A93C-8872-4300-BD66-3FDD9EC5CC69}"/>
+    <hyperlink ref="C78" r:id="rId47" xr:uid="{060F7AA6-4151-4640-9125-EB05725D5C4E}"/>
+    <hyperlink ref="C71" r:id="rId48" xr:uid="{2A014FF4-6899-437D-9B86-4081802651C4}"/>
+    <hyperlink ref="C62" r:id="rId49" xr:uid="{222265FC-E132-423E-B05E-78435D160A16}"/>
+    <hyperlink ref="C56" r:id="rId50" xr:uid="{EB9E6D4D-614F-426A-B561-DD86A9C73718}"/>
+    <hyperlink ref="C55" r:id="rId51" xr:uid="{49603C16-1494-480F-AF14-8DD65509D0A0}"/>
+    <hyperlink ref="C54" r:id="rId52" xr:uid="{EE2BA59D-84E1-4A3C-86BD-E9E0C33D7DFB}"/>
+    <hyperlink ref="C45" r:id="rId53" xr:uid="{642DD3F3-46F4-448D-BD86-703F11F37A10}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finalised scraper_links_hist, new concept for what data to store how etc. in readme_notes
</commit_message>
<xml_diff>
--- a/union_data.xlsx
+++ b/union_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexBusch\Documents\GitHub\industrial_action\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BDFDB0-1C28-4208-B79B-4275FD663965}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F025B5D-B855-4765-A637-6D4CD88E2D15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10500" xr2:uid="{55DB6E5A-4C35-45C3-9C4F-265E93AFAEF7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="504">
   <si>
     <t>U-Union</t>
   </si>
@@ -1530,6 +1530,15 @@
   </si>
   <si>
     <t xml:space="preserve">Kiel </t>
+  </si>
+  <si>
+    <t>https://www.igmetall.de/presse/pressemitteilungen/</t>
+  </si>
+  <si>
+    <t>https://rosenheim.igmetall.de/aktuelles/</t>
+  </si>
+  <si>
+    <t>https://rendsburg.igmetall.de/aktuell/</t>
   </si>
 </sst>
 </file>
@@ -1895,7 +1904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF38B2E-D1B8-4839-8784-A9099D704EE1}">
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
       <selection activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>
@@ -4283,8 +4292,8 @@
       <c r="B107" t="s">
         <v>3</v>
       </c>
-      <c r="C107" t="s">
-        <v>275</v>
+      <c r="C107" s="1" t="s">
+        <v>503</v>
       </c>
       <c r="D107" t="s">
         <v>163</v>
@@ -4372,8 +4381,8 @@
       <c r="B111" t="s">
         <v>3</v>
       </c>
-      <c r="C111" t="s">
-        <v>169</v>
+      <c r="C111" s="1" t="s">
+        <v>502</v>
       </c>
       <c r="D111" t="s">
         <v>170</v>
@@ -5230,7 +5239,7 @@
         <v>414</v>
       </c>
       <c r="E148" t="s">
-        <v>440</v>
+        <v>13</v>
       </c>
       <c r="G148" t="s">
         <v>322</v>
@@ -5244,7 +5253,7 @@
         <v>3</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>432</v>
+        <v>501</v>
       </c>
       <c r="D149" t="s">
         <v>416</v>
@@ -5326,14 +5335,16 @@
     <hyperlink ref="C125" r:id="rId60" xr:uid="{18B4DFA8-35D8-4799-8D53-71C3CC5CCF65}"/>
     <hyperlink ref="C145" r:id="rId61" xr:uid="{4D949951-0104-4AB8-8B43-7AD5FC2029D8}"/>
     <hyperlink ref="C144" r:id="rId62" xr:uid="{96900B3C-9A82-4FCA-A99B-DA7956113148}"/>
-    <hyperlink ref="C149" r:id="rId63" xr:uid="{D0421B36-0296-4376-A390-5741E7654B52}"/>
-    <hyperlink ref="C146" r:id="rId64" xr:uid="{B084E596-0EAD-4841-8581-A7F1A096F217}"/>
-    <hyperlink ref="C147" r:id="rId65" xr:uid="{C920FBFA-CB69-4F7D-8EA6-D7420E7EF080}"/>
-    <hyperlink ref="C46" r:id="rId66" xr:uid="{03EEA6E0-6E61-41DA-A8CD-C97AD4F67B20}"/>
-    <hyperlink ref="C101" r:id="rId67" xr:uid="{6A37F3EC-DBAD-4730-9D2E-C8FE8F5BE4B2}"/>
-    <hyperlink ref="C80" r:id="rId68" xr:uid="{EB7B19AD-7F59-4E34-9419-EDE502C0635E}"/>
-    <hyperlink ref="C47" r:id="rId69" xr:uid="{5D6E3871-87ED-4BDF-9D0C-DCFB58CFC5D4}"/>
-    <hyperlink ref="C89" r:id="rId70" xr:uid="{67EA448E-10ED-469A-B7F9-17E332E689A9}"/>
+    <hyperlink ref="C146" r:id="rId63" xr:uid="{B084E596-0EAD-4841-8581-A7F1A096F217}"/>
+    <hyperlink ref="C147" r:id="rId64" xr:uid="{C920FBFA-CB69-4F7D-8EA6-D7420E7EF080}"/>
+    <hyperlink ref="C46" r:id="rId65" xr:uid="{03EEA6E0-6E61-41DA-A8CD-C97AD4F67B20}"/>
+    <hyperlink ref="C101" r:id="rId66" xr:uid="{6A37F3EC-DBAD-4730-9D2E-C8FE8F5BE4B2}"/>
+    <hyperlink ref="C80" r:id="rId67" xr:uid="{EB7B19AD-7F59-4E34-9419-EDE502C0635E}"/>
+    <hyperlink ref="C47" r:id="rId68" xr:uid="{5D6E3871-87ED-4BDF-9D0C-DCFB58CFC5D4}"/>
+    <hyperlink ref="C89" r:id="rId69" xr:uid="{67EA448E-10ED-469A-B7F9-17E332E689A9}"/>
+    <hyperlink ref="C149" r:id="rId70" xr:uid="{465F8FB3-C176-4845-A64F-F9946A0C557A}"/>
+    <hyperlink ref="C111" r:id="rId71" xr:uid="{A7DFF63B-DA63-4DFC-A171-0C3E120A1F53}"/>
+    <hyperlink ref="C107" r:id="rId72" xr:uid="{E91AADE8-F04D-4AF5-9F90-67D915C75480}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>